<commit_message>
edit processa_dados: adiciona a função separa_namostra
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -1,22 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ilumcnpem-my.sharepoint.com/personal/joao25006_ilum_cnpem_br/Documents/VS code/PCD_Placa_de_ELISA/No-Stress_ELISA/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_7567781D39B9978B6218F0B19B069447DC6C65F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8230D99A-8BA7-4214-BD67-3B86A5BC8F16}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="100" windowWidth="9000" windowHeight="8000"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
     <sheet name="Results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" calcMode="auto"/>
+  <calcPr calcId="191029"/>
   <webPublishing codePage="1250"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="230">
   <si>
     <t>Method</t>
   </si>
@@ -703,16 +722,19 @@
   </si>
   <si>
     <t>Sample 1.96</t>
+  </si>
+  <si>
+    <t>A415</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="#####0.000"/>
+    <numFmt numFmtId="164" formatCode="#####0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -725,6 +747,22 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -747,22 +785,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1063,25 +1120,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Header"/>
   <dimension ref="B2:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" defaultGridColor="0" colorId="64" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.83333" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1089,7 +1144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1105,12 +1160,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -1118,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1181,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -1134,12 +1189,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1147,7 +1202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -1155,7 +1210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1218,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>20</v>
       </c>
@@ -1171,7 +1226,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -1179,7 +1234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -1187,7 +1242,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>26</v>
       </c>
@@ -1195,12 +1250,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>29</v>
       </c>
@@ -1208,7 +1263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>31</v>
       </c>
@@ -1216,7 +1271,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>32</v>
       </c>
@@ -1230,17 +1285,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Results"/>
-  <dimension ref="B2:D98"/>
+  <dimension ref="B2:E98"/>
   <sheetViews>
-    <sheetView defaultGridColor="0" colorId="64" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="9.1640625" style="6"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1250,8 +1308,11 @@
       <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="2:4">
+      <c r="E2" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>37</v>
       </c>
@@ -1259,10 +1320,14 @@
         <v>38</v>
       </c>
       <c r="D3" s="3">
-        <v>0.425</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3-0.023</f>
+        <v>0.40199999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>39</v>
       </c>
@@ -1270,10 +1335,14 @@
         <v>40</v>
       </c>
       <c r="D4" s="3">
-        <v>0.397</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E67" si="0">D4-0.023</f>
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>41</v>
       </c>
@@ -1281,10 +1350,14 @@
         <v>42</v>
       </c>
       <c r="D5" s="3">
-        <v>0.205</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>43</v>
       </c>
@@ -1292,10 +1365,14 @@
         <v>44</v>
       </c>
       <c r="D6" s="3">
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>45</v>
       </c>
@@ -1303,10 +1380,14 @@
         <v>46</v>
       </c>
       <c r="D7" s="3">
-        <v>0.392</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>47</v>
       </c>
@@ -1314,10 +1395,14 @@
         <v>48</v>
       </c>
       <c r="D8" s="3">
-        <v>0.422</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39899999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>49</v>
       </c>
@@ -1327,8 +1412,12 @@
       <c r="D9" s="3">
         <v>0.432</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40899999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>51</v>
       </c>
@@ -1336,10 +1425,14 @@
         <v>52</v>
       </c>
       <c r="D10" s="3">
-        <v>0.047</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -1347,10 +1440,14 @@
         <v>54</v>
       </c>
       <c r="D11" s="3">
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -1360,8 +1457,12 @@
       <c r="D12" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="2:4">
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>57</v>
       </c>
@@ -1369,10 +1470,14 @@
         <v>58</v>
       </c>
       <c r="D13" s="3">
-        <v>0.052</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>59</v>
       </c>
@@ -1380,10 +1485,14 @@
         <v>60</v>
       </c>
       <c r="D14" s="3">
-        <v>0.051</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>61</v>
       </c>
@@ -1391,10 +1500,14 @@
         <v>62</v>
       </c>
       <c r="D15" s="3">
-        <v>0.417</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39399999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>63</v>
       </c>
@@ -1404,8 +1517,12 @@
       <c r="D16" s="3">
         <v>0.378</v>
       </c>
-    </row>
-    <row r="17" spans="2:4">
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>65</v>
       </c>
@@ -1413,10 +1530,14 @@
         <v>66</v>
       </c>
       <c r="D17" s="3">
-        <v>0.208</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>67</v>
       </c>
@@ -1424,10 +1545,14 @@
         <v>68</v>
       </c>
       <c r="D18" s="3">
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>69</v>
       </c>
@@ -1435,10 +1560,14 @@
         <v>70</v>
       </c>
       <c r="D19" s="3">
-        <v>0.478</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45499999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>71</v>
       </c>
@@ -1446,10 +1575,14 @@
         <v>72</v>
       </c>
       <c r="D20" s="3">
-        <v>0.415</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39199999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>73</v>
       </c>
@@ -1459,8 +1592,12 @@
       <c r="D21" s="3">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="22" spans="2:4">
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34699999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>75</v>
       </c>
@@ -1468,10 +1605,14 @@
         <v>76</v>
       </c>
       <c r="D22" s="3">
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="0"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>77</v>
       </c>
@@ -1479,10 +1620,14 @@
         <v>78</v>
       </c>
       <c r="D23" s="3">
-        <v>0.048</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>79</v>
       </c>
@@ -1490,10 +1635,14 @@
         <v>80</v>
       </c>
       <c r="D24" s="3">
-        <v>0.043</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>81</v>
       </c>
@@ -1501,10 +1650,14 @@
         <v>82</v>
       </c>
       <c r="D25" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>83</v>
       </c>
@@ -1512,10 +1665,14 @@
         <v>84</v>
       </c>
       <c r="D26" s="3">
-        <v>0.052</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>85</v>
       </c>
@@ -1523,10 +1680,14 @@
         <v>86</v>
       </c>
       <c r="D27" s="3">
-        <v>0.447</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>87</v>
       </c>
@@ -1534,10 +1695,14 @@
         <v>88</v>
       </c>
       <c r="D28" s="3">
-        <v>0.382</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="0"/>
+        <v>0.35899999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>89</v>
       </c>
@@ -1545,10 +1710,14 @@
         <v>90</v>
       </c>
       <c r="D29" s="3">
-        <v>0.206</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="0"/>
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>91</v>
       </c>
@@ -1556,10 +1725,14 @@
         <v>92</v>
       </c>
       <c r="D30" s="3">
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="0"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>93</v>
       </c>
@@ -1567,10 +1740,14 @@
         <v>94</v>
       </c>
       <c r="D31" s="3">
-        <v>0.465</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>95</v>
       </c>
@@ -1578,10 +1755,14 @@
         <v>96</v>
       </c>
       <c r="D32" s="3">
-        <v>0.418</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39499999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>97</v>
       </c>
@@ -1589,10 +1770,14 @@
         <v>98</v>
       </c>
       <c r="D33" s="3">
-        <v>0.473</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="E33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>99</v>
       </c>
@@ -1600,10 +1785,14 @@
         <v>100</v>
       </c>
       <c r="D34" s="3">
-        <v>0.048</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E34" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>101</v>
       </c>
@@ -1611,10 +1800,14 @@
         <v>102</v>
       </c>
       <c r="D35" s="3">
-        <v>0.047</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E35" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>103</v>
       </c>
@@ -1622,10 +1815,14 @@
         <v>104</v>
       </c>
       <c r="D36" s="3">
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E36" s="5">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>105</v>
       </c>
@@ -1633,10 +1830,14 @@
         <v>106</v>
       </c>
       <c r="D37" s="3">
-        <v>0.043</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E37" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>107</v>
       </c>
@@ -1644,10 +1845,14 @@
         <v>108</v>
       </c>
       <c r="D38" s="3">
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E38" s="5">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>109</v>
       </c>
@@ -1655,10 +1860,14 @@
         <v>110</v>
       </c>
       <c r="D39" s="3">
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E39" s="5">
+        <f t="shared" si="0"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>111</v>
       </c>
@@ -1666,10 +1875,14 @@
         <v>112</v>
       </c>
       <c r="D40" s="3">
-        <v>0.045</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E40" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>113</v>
       </c>
@@ -1677,10 +1890,14 @@
         <v>114</v>
       </c>
       <c r="D41" s="3">
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E41" s="5">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>115</v>
       </c>
@@ -1688,10 +1905,14 @@
         <v>116</v>
       </c>
       <c r="D42" s="3">
-        <v>0.041</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E42" s="5">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>117</v>
       </c>
@@ -1699,10 +1920,14 @@
         <v>118</v>
       </c>
       <c r="D43" s="3">
-        <v>0.043</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E43" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>119</v>
       </c>
@@ -1710,10 +1935,14 @@
         <v>120</v>
       </c>
       <c r="D44" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E44" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>121</v>
       </c>
@@ -1721,10 +1950,14 @@
         <v>122</v>
       </c>
       <c r="D45" s="3">
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E45" s="5">
+        <f t="shared" si="0"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>123</v>
       </c>
@@ -1732,10 +1965,14 @@
         <v>124</v>
       </c>
       <c r="D46" s="3">
-        <v>0.048</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E46" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>125</v>
       </c>
@@ -1743,10 +1980,14 @@
         <v>126</v>
       </c>
       <c r="D47" s="3">
-        <v>0.047</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E47" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>127</v>
       </c>
@@ -1754,10 +1995,14 @@
         <v>128</v>
       </c>
       <c r="D48" s="3">
-        <v>0.045</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E48" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>129</v>
       </c>
@@ -1765,10 +2010,14 @@
         <v>130</v>
       </c>
       <c r="D49" s="3">
-        <v>0.047</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E49" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>131</v>
       </c>
@@ -1778,8 +2027,12 @@
       <c r="D50" s="3">
         <v>0.123</v>
       </c>
-    </row>
-    <row r="51" spans="2:4">
+      <c r="E50" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>133</v>
       </c>
@@ -1787,10 +2040,14 @@
         <v>134</v>
       </c>
       <c r="D51" s="3">
-        <v>0.043</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E51" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>135</v>
       </c>
@@ -1798,10 +2055,14 @@
         <v>136</v>
       </c>
       <c r="D52" s="3">
-        <v>0.043</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E52" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>137</v>
       </c>
@@ -1809,10 +2070,14 @@
         <v>138</v>
       </c>
       <c r="D53" s="3">
-        <v>0.043</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E53" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>139</v>
       </c>
@@ -1820,10 +2085,14 @@
         <v>140</v>
       </c>
       <c r="D54" s="3">
-        <v>0.043</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="E54" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>141</v>
       </c>
@@ -1831,10 +2100,14 @@
         <v>142</v>
       </c>
       <c r="D55" s="3">
-        <v>0.045</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E55" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>143</v>
       </c>
@@ -1842,10 +2115,14 @@
         <v>144</v>
       </c>
       <c r="D56" s="3">
-        <v>0.045</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E56" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>145</v>
       </c>
@@ -1853,10 +2130,14 @@
         <v>146</v>
       </c>
       <c r="D57" s="3">
-        <v>0.053</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E57" s="5">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>147</v>
       </c>
@@ -1864,10 +2145,14 @@
         <v>148</v>
       </c>
       <c r="D58" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E58" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>149</v>
       </c>
@@ -1875,10 +2160,14 @@
         <v>150</v>
       </c>
       <c r="D59" s="3">
-        <v>0.052</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E59" s="5">
+        <f t="shared" si="0"/>
+        <v>2.8999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>151</v>
       </c>
@@ -1886,10 +2175,14 @@
         <v>152</v>
       </c>
       <c r="D60" s="3">
-        <v>0.053</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E60" s="5">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>153</v>
       </c>
@@ -1897,10 +2190,14 @@
         <v>154</v>
       </c>
       <c r="D61" s="3">
-        <v>0.048</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E61" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>155</v>
       </c>
@@ -1908,10 +2205,14 @@
         <v>156</v>
       </c>
       <c r="D62" s="3">
-        <v>0.048</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E62" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>157</v>
       </c>
@@ -1921,8 +2222,12 @@
       <c r="D63" s="3">
         <v>1.091</v>
       </c>
-    </row>
-    <row r="64" spans="2:4">
+      <c r="E63" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0680000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>159</v>
       </c>
@@ -1930,10 +2235,14 @@
         <v>160</v>
       </c>
       <c r="D64" s="3">
-        <v>0.447</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E64" s="5">
+        <f t="shared" si="0"/>
+        <v>0.42399999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>161</v>
       </c>
@@ -1941,10 +2250,14 @@
         <v>162</v>
       </c>
       <c r="D65" s="3">
-        <v>0.494</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="E65" s="5">
+        <f t="shared" si="0"/>
+        <v>0.47099999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>163</v>
       </c>
@@ -1952,10 +2265,14 @@
         <v>164</v>
       </c>
       <c r="D66" s="3">
-        <v>0.044</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="E66" s="5">
+        <f t="shared" si="0"/>
+        <v>2.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>165</v>
       </c>
@@ -1965,8 +2282,12 @@
       <c r="D67" s="3">
         <v>1.288</v>
       </c>
-    </row>
-    <row r="68" spans="2:4">
+      <c r="E67" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2650000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -1974,10 +2295,14 @@
         <v>168</v>
       </c>
       <c r="D68" s="3">
-        <v>0.56</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E68" s="5">
+        <f t="shared" ref="E68:E98" si="1">D68-0.023</f>
+        <v>0.53700000000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>169</v>
       </c>
@@ -1987,8 +2312,12 @@
       <c r="D69" s="3">
         <v>1.419</v>
       </c>
-    </row>
-    <row r="70" spans="2:4">
+      <c r="E69" s="5">
+        <f t="shared" si="1"/>
+        <v>1.3960000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>171</v>
       </c>
@@ -1996,10 +2325,14 @@
         <v>172</v>
       </c>
       <c r="D70" s="3">
-        <v>0.053</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E70" s="5">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>173</v>
       </c>
@@ -2009,8 +2342,12 @@
       <c r="D71" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="72" spans="2:4">
+      <c r="E71" s="5">
+        <f t="shared" si="1"/>
+        <v>2.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>175</v>
       </c>
@@ -2018,10 +2355,14 @@
         <v>176</v>
       </c>
       <c r="D72" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E72" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>177</v>
       </c>
@@ -2029,10 +2370,14 @@
         <v>178</v>
       </c>
       <c r="D73" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E73" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>179</v>
       </c>
@@ -2040,10 +2385,14 @@
         <v>180</v>
       </c>
       <c r="D74" s="3">
-        <v>0.047</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4">
+        <v>4.7E-2</v>
+      </c>
+      <c r="E74" s="5">
+        <f t="shared" si="1"/>
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>181</v>
       </c>
@@ -2051,10 +2400,14 @@
         <v>182</v>
       </c>
       <c r="D75" s="3">
-        <v>1.128</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4">
+        <v>1.1279999999999999</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" si="1"/>
+        <v>1.105</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>183</v>
       </c>
@@ -2062,10 +2415,14 @@
         <v>184</v>
       </c>
       <c r="D76" s="3">
-        <v>0.446</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" si="1"/>
+        <v>0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>185</v>
       </c>
@@ -2075,8 +2432,12 @@
       <c r="D77" s="3">
         <v>0.497</v>
       </c>
-    </row>
-    <row r="78" spans="2:4">
+      <c r="E77" s="5">
+        <f t="shared" si="1"/>
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>187</v>
       </c>
@@ -2084,10 +2445,14 @@
         <v>188</v>
       </c>
       <c r="D78" s="3">
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E78" s="5">
+        <f t="shared" si="1"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>189</v>
       </c>
@@ -2095,10 +2460,14 @@
         <v>190</v>
       </c>
       <c r="D79" s="3">
-        <v>1.314</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="E79" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2910000000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>191</v>
       </c>
@@ -2106,10 +2475,14 @@
         <v>192</v>
       </c>
       <c r="D80" s="3">
-        <v>0.567</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="E80" s="5">
+        <f t="shared" si="1"/>
+        <v>0.54399999999999993</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>193</v>
       </c>
@@ -2119,8 +2492,12 @@
       <c r="D81" s="3">
         <v>1.492</v>
       </c>
-    </row>
-    <row r="82" spans="2:4">
+      <c r="E81" s="5">
+        <f t="shared" si="1"/>
+        <v>1.4690000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>195</v>
       </c>
@@ -2128,10 +2505,14 @@
         <v>196</v>
       </c>
       <c r="D82" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E82" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>197</v>
       </c>
@@ -2141,8 +2522,12 @@
       <c r="D83" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="84" spans="2:4">
+      <c r="E83" s="5">
+        <f t="shared" si="1"/>
+        <v>2.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>199</v>
       </c>
@@ -2150,10 +2535,14 @@
         <v>200</v>
       </c>
       <c r="D84" s="3">
-        <v>0.046</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E84" s="5">
+        <f t="shared" si="1"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>201</v>
       </c>
@@ -2161,10 +2550,14 @@
         <v>202</v>
       </c>
       <c r="D85" s="3">
-        <v>0.048</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E85" s="5">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>203</v>
       </c>
@@ -2172,10 +2565,14 @@
         <v>204</v>
       </c>
       <c r="D86" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E86" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>205</v>
       </c>
@@ -2183,10 +2580,14 @@
         <v>206</v>
       </c>
       <c r="D87" s="3">
-        <v>1.14</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="E87" s="5">
+        <f t="shared" si="1"/>
+        <v>1.117</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>207</v>
       </c>
@@ -2194,10 +2595,14 @@
         <v>208</v>
       </c>
       <c r="D88" s="3">
-        <v>0.481</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="E88" s="5">
+        <f t="shared" si="1"/>
+        <v>0.45799999999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>209</v>
       </c>
@@ -2207,8 +2612,12 @@
       <c r="D89" s="3">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="90" spans="2:4">
+      <c r="E89" s="5">
+        <f t="shared" si="1"/>
+        <v>0.46699999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>211</v>
       </c>
@@ -2216,10 +2625,14 @@
         <v>212</v>
       </c>
       <c r="D90" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E90" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>213</v>
       </c>
@@ -2227,10 +2640,14 @@
         <v>214</v>
       </c>
       <c r="D91" s="3">
-        <v>1.318</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="E91" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2950000000000002</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>215</v>
       </c>
@@ -2238,10 +2655,14 @@
         <v>216</v>
       </c>
       <c r="D92" s="3">
-        <v>0.542</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="E92" s="5">
+        <f t="shared" si="1"/>
+        <v>0.51900000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>217</v>
       </c>
@@ -2249,10 +2670,14 @@
         <v>218</v>
       </c>
       <c r="D93" s="3">
-        <v>1.412</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4">
+        <v>1.4119999999999999</v>
+      </c>
+      <c r="E93" s="5">
+        <f t="shared" si="1"/>
+        <v>1.389</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>219</v>
       </c>
@@ -2260,10 +2685,14 @@
         <v>220</v>
       </c>
       <c r="D94" s="3">
-        <v>0.055</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E94" s="5">
+        <f t="shared" si="1"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>221</v>
       </c>
@@ -2271,10 +2700,14 @@
         <v>222</v>
       </c>
       <c r="D95" s="3">
-        <v>0.057</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E95" s="5">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>223</v>
       </c>
@@ -2284,8 +2717,12 @@
       <c r="D96" s="3">
         <v>0.107</v>
       </c>
-    </row>
-    <row r="97" spans="2:4">
+      <c r="E96" s="5">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999991E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>225</v>
       </c>
@@ -2293,10 +2730,14 @@
         <v>226</v>
       </c>
       <c r="D97" s="3">
-        <v>0.049</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E97" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>227</v>
       </c>
@@ -2304,7 +2745,11 @@
         <v>228</v>
       </c>
       <c r="D98" s="3">
-        <v>0.134</v>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="E98" s="5">
+        <f t="shared" si="1"/>
+        <v>0.11100000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit separa_namostras: faz o código funcioar para várias absorbânicas
</commit_message>
<xml_diff>
--- a/Teste.xlsx
+++ b/Teste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ilumcnpem-my.sharepoint.com/personal/joao25006_ilum_cnpem_br/Documents/VS code/PCD_Placa_de_ELISA/No-Stress_ELISA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_7567781D39B9978B6218F0B19B069447DC6C65F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8230D99A-8BA7-4214-BD67-3B86A5BC8F16}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_7567781D39B9978B6218F0B19B069447DC6C65F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA878011-6E98-4851-9217-3E5E01B748A3}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1289,8 +1289,8 @@
   <sheetPr codeName="Results"/>
   <dimension ref="B2:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1323,8 +1323,8 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="E3" s="5">
-        <f>D3-0.023</f>
-        <v>0.40199999999999997</v>
+        <f ca="1" xml:space="preserve"> 1 + RANDBETWEEN(1, 10) / 10</f>
+        <v>1.4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
@@ -1338,8 +1338,8 @@
         <v>0.39700000000000002</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E67" si="0">D4-0.023</f>
-        <v>0.374</v>
+        <f t="shared" ref="E4:E67" ca="1" si="0" xml:space="preserve"> 1 + RANDBETWEEN(1, 10) / 10</f>
+        <v>1.8</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
@@ -1353,8 +1353,8 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>0.182</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
@@ -1368,8 +1368,8 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>2.0999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
@@ -1383,8 +1383,8 @@
         <v>0.39200000000000002</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>0.36899999999999999</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
@@ -1398,8 +1398,8 @@
         <v>0.42199999999999999</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>0.39899999999999997</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
@@ -1413,8 +1413,8 @@
         <v>0.432</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.40899999999999997</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
@@ -1428,8 +1428,8 @@
         <v>4.7E-2</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
@@ -1443,8 +1443,8 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
@@ -1458,8 +1458,8 @@
         <v>0.05</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>2.7000000000000003E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
@@ -1473,8 +1473,8 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="0"/>
-        <v>2.8999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
@@ -1488,8 +1488,8 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="0"/>
-        <v>2.7999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
@@ -1503,8 +1503,8 @@
         <v>0.41699999999999998</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="0"/>
-        <v>0.39399999999999996</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
@@ -1518,8 +1518,8 @@
         <v>0.378</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="0"/>
-        <v>0.35499999999999998</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
@@ -1533,8 +1533,8 @@
         <v>0.20799999999999999</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="0"/>
-        <v>0.185</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
@@ -1548,8 +1548,8 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="0"/>
-        <v>2.0999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
@@ -1563,8 +1563,8 @@
         <v>0.47799999999999998</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="0"/>
-        <v>0.45499999999999996</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
@@ -1578,8 +1578,8 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="0"/>
-        <v>0.39199999999999996</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
@@ -1593,8 +1593,8 @@
         <v>0.37</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="0"/>
-        <v>0.34699999999999998</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
@@ -1608,8 +1608,8 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
@@ -1623,8 +1623,8 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
@@ -1638,8 +1638,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
@@ -1653,8 +1653,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="0"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
@@ -1668,8 +1668,8 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="0"/>
-        <v>2.8999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
@@ -1683,8 +1683,8 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" si="0"/>
-        <v>0.42399999999999999</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
@@ -1698,8 +1698,8 @@
         <v>0.38200000000000001</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="0"/>
-        <v>0.35899999999999999</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
@@ -1713,8 +1713,8 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="0"/>
-        <v>0.183</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
@@ -1728,8 +1728,8 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
@@ -1743,8 +1743,8 @@
         <v>0.46500000000000002</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="0"/>
-        <v>0.442</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
@@ -1758,8 +1758,8 @@
         <v>0.41799999999999998</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" si="0"/>
-        <v>0.39499999999999996</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
@@ -1773,8 +1773,8 @@
         <v>0.47299999999999998</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
@@ -1788,8 +1788,8 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E34" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
@@ -1803,8 +1803,8 @@
         <v>4.7E-2</v>
       </c>
       <c r="E35" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
@@ -1818,8 +1818,8 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="0"/>
-        <v>2.0999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
@@ -1833,8 +1833,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
@@ -1848,8 +1848,8 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="0"/>
-        <v>2.0999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
@@ -1863,8 +1863,8 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
@@ -1878,8 +1878,8 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="0"/>
-        <v>2.1999999999999999E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
@@ -1893,8 +1893,8 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="0"/>
-        <v>2.0999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
@@ -1908,8 +1908,8 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8000000000000002E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -1923,8 +1923,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
@@ -1938,8 +1938,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="0"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.35">
@@ -1953,8 +1953,8 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="0"/>
-        <v>2.3E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.35">
@@ -1968,8 +1968,8 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.35">
@@ -1983,8 +1983,8 @@
         <v>4.7E-2</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.35">
@@ -1998,8 +1998,8 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E48" s="5">
-        <f t="shared" si="0"/>
-        <v>2.1999999999999999E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.35">
@@ -2013,8 +2013,8 @@
         <v>4.7E-2</v>
       </c>
       <c r="E49" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
@@ -2028,8 +2028,8 @@
         <v>0.123</v>
       </c>
       <c r="E50" s="5">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
@@ -2043,8 +2043,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E51" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
@@ -2058,8 +2058,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E52" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.35">
@@ -2073,8 +2073,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E53" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.35">
@@ -2088,8 +2088,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E54" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9999999999999997E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.35">
@@ -2103,8 +2103,8 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E55" s="5">
-        <f t="shared" si="0"/>
-        <v>2.1999999999999999E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.35">
@@ -2118,8 +2118,8 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E56" s="5">
-        <f t="shared" si="0"/>
-        <v>2.1999999999999999E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.35">
@@ -2133,8 +2133,8 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="E57" s="5">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.35">
@@ -2148,8 +2148,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E58" s="5">
-        <f t="shared" si="0"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
@@ -2163,8 +2163,8 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="E59" s="5">
-        <f t="shared" si="0"/>
-        <v>2.8999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
@@ -2178,8 +2178,8 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="E60" s="5">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.35">
@@ -2193,8 +2193,8 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E61" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.35">
@@ -2208,8 +2208,8 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E62" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.35">
@@ -2223,8 +2223,8 @@
         <v>1.091</v>
       </c>
       <c r="E63" s="5">
-        <f t="shared" si="0"/>
-        <v>1.0680000000000001</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.35">
@@ -2238,8 +2238,8 @@
         <v>0.44700000000000001</v>
       </c>
       <c r="E64" s="5">
-        <f t="shared" si="0"/>
-        <v>0.42399999999999999</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.35">
@@ -2253,8 +2253,8 @@
         <v>0.49399999999999999</v>
       </c>
       <c r="E65" s="5">
-        <f t="shared" si="0"/>
-        <v>0.47099999999999997</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.35">
@@ -2268,8 +2268,8 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="E66" s="5">
-        <f t="shared" si="0"/>
-        <v>2.0999999999999998E-2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.35">
@@ -2283,8 +2283,8 @@
         <v>1.288</v>
       </c>
       <c r="E67" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2650000000000001</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.35">
@@ -2298,8 +2298,8 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="E68" s="5">
-        <f t="shared" ref="E68:E98" si="1">D68-0.023</f>
-        <v>0.53700000000000003</v>
+        <f t="shared" ref="E68:E98" ca="1" si="1" xml:space="preserve"> 1 + RANDBETWEEN(1, 10) / 10</f>
+        <v>1.7</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.35">
@@ -2313,8 +2313,8 @@
         <v>1.419</v>
       </c>
       <c r="E69" s="5">
-        <f t="shared" si="1"/>
-        <v>1.3960000000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.35">
@@ -2328,8 +2328,8 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="E70" s="5">
-        <f t="shared" si="1"/>
-        <v>0.03</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.4</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.35">
@@ -2343,8 +2343,8 @@
         <v>0.05</v>
       </c>
       <c r="E71" s="5">
-        <f t="shared" si="1"/>
-        <v>2.7000000000000003E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.4</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.35">
@@ -2358,8 +2358,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E72" s="5">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.35">
@@ -2373,8 +2373,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E73" s="5">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.35">
@@ -2388,8 +2388,8 @@
         <v>4.7E-2</v>
       </c>
       <c r="E74" s="5">
-        <f t="shared" si="1"/>
-        <v>2.4E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.35">
@@ -2403,8 +2403,8 @@
         <v>1.1279999999999999</v>
       </c>
       <c r="E75" s="5">
-        <f t="shared" si="1"/>
-        <v>1.105</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.35">
@@ -2418,8 +2418,8 @@
         <v>0.44600000000000001</v>
       </c>
       <c r="E76" s="5">
-        <f t="shared" si="1"/>
-        <v>0.42299999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.35">
@@ -2433,8 +2433,8 @@
         <v>0.497</v>
       </c>
       <c r="E77" s="5">
-        <f t="shared" si="1"/>
-        <v>0.47399999999999998</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.35">
@@ -2448,8 +2448,8 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E78" s="5">
-        <f t="shared" si="1"/>
-        <v>2.3E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.35">
@@ -2463,8 +2463,8 @@
         <v>1.3140000000000001</v>
       </c>
       <c r="E79" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2910000000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.35">
@@ -2478,8 +2478,8 @@
         <v>0.56699999999999995</v>
       </c>
       <c r="E80" s="5">
-        <f t="shared" si="1"/>
-        <v>0.54399999999999993</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.35">
@@ -2493,8 +2493,8 @@
         <v>1.492</v>
       </c>
       <c r="E81" s="5">
-        <f t="shared" si="1"/>
-        <v>1.4690000000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.35">
@@ -2508,8 +2508,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E82" s="5">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.35">
@@ -2523,8 +2523,8 @@
         <v>0.05</v>
       </c>
       <c r="E83" s="5">
-        <f t="shared" si="1"/>
-        <v>2.7000000000000003E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.35">
@@ -2538,8 +2538,8 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="E84" s="5">
-        <f t="shared" si="1"/>
-        <v>2.3E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.35">
@@ -2553,8 +2553,8 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E85" s="5">
-        <f t="shared" si="1"/>
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.35">
@@ -2568,8 +2568,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E86" s="5">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.35">
@@ -2583,8 +2583,8 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="E87" s="5">
-        <f t="shared" si="1"/>
-        <v>1.117</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.35">
@@ -2598,8 +2598,8 @@
         <v>0.48099999999999998</v>
       </c>
       <c r="E88" s="5">
-        <f t="shared" si="1"/>
-        <v>0.45799999999999996</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.35">
@@ -2613,8 +2613,8 @@
         <v>0.49</v>
       </c>
       <c r="E89" s="5">
-        <f t="shared" si="1"/>
-        <v>0.46699999999999997</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3</v>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.35">
@@ -2628,8 +2628,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E90" s="5">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.35">
@@ -2643,8 +2643,8 @@
         <v>1.3180000000000001</v>
       </c>
       <c r="E91" s="5">
-        <f t="shared" si="1"/>
-        <v>1.2950000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.8</v>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.35">
@@ -2658,8 +2658,8 @@
         <v>0.54200000000000004</v>
       </c>
       <c r="E92" s="5">
-        <f t="shared" si="1"/>
-        <v>0.51900000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.35">
@@ -2673,8 +2673,8 @@
         <v>1.4119999999999999</v>
       </c>
       <c r="E93" s="5">
-        <f t="shared" si="1"/>
-        <v>1.389</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6</v>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.35">
@@ -2688,8 +2688,8 @@
         <v>5.5E-2</v>
       </c>
       <c r="E94" s="5">
-        <f t="shared" si="1"/>
-        <v>3.2000000000000001E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.35">
@@ -2703,8 +2703,8 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="E95" s="5">
-        <f t="shared" si="1"/>
-        <v>3.4000000000000002E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.35">
@@ -2718,8 +2718,8 @@
         <v>0.107</v>
       </c>
       <c r="E96" s="5">
-        <f t="shared" si="1"/>
-        <v>8.3999999999999991E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.35">
@@ -2733,8 +2733,8 @@
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="E97" s="5">
-        <f t="shared" si="1"/>
-        <v>2.6000000000000002E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.35">
@@ -2748,8 +2748,8 @@
         <v>0.13400000000000001</v>
       </c>
       <c r="E98" s="5">
-        <f t="shared" si="1"/>
-        <v>0.11100000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>